<commit_message>
Major improvements to the algorithm, making it more general
</commit_message>
<xml_diff>
--- a/GoogleVision/src/tables/Vergiler14.xlsx
+++ b/GoogleVision/src/tables/Vergiler14.xlsx
@@ -38,28 +38,28 @@
     <t>Toplam</t>
   </si>
   <si>
-    <t>EF : 22021</t>
+    <t>14/07/2022</t>
   </si>
   <si>
-    <t>SEBA GRUF GIDA ELEKTRİK</t>
+    <t>MIGROS TICARET A.S.</t>
   </si>
   <si>
-    <t>000021</t>
+    <t>0506</t>
   </si>
   <si>
-    <t>ETIMESGUT</t>
+    <t xml:space="preserve">BUYUK MUKELLEFLER </t>
   </si>
   <si>
-    <t>7570730929</t>
+    <t>6220529513</t>
   </si>
   <si>
-    <t>0.81</t>
+    <t>31.11</t>
   </si>
   <si>
-    <t>10.19</t>
+    <t>172.83</t>
   </si>
   <si>
-    <t>11.00</t>
+    <t>203.94</t>
   </si>
 </sst>
 </file>

</xml_diff>